<commit_message>
tabla con resultados + script SimulacionMOdelos
</commit_message>
<xml_diff>
--- a/ResultadosSimulaciones.xlsx
+++ b/ResultadosSimulaciones.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>REGRESIÓN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Tasa de Aprendizaje</t>
   </si>
@@ -40,6 +37,15 @@
   </si>
   <si>
     <t>0.05</t>
+  </si>
+  <si>
+    <t>DATOS REGRESIÓN MULTIPLE</t>
+  </si>
+  <si>
+    <t>TABLA1</t>
+  </si>
+  <si>
+    <t>TABLA2</t>
   </si>
 </sst>
 </file>
@@ -49,7 +55,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,11 +65,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -83,24 +94,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -112,28 +106,11 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -145,32 +122,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -474,176 +449,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="E2" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>0.1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" s="7">
         <v>19878.250100000001</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="7">
+        <v>28163.052800000001</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="7">
         <v>19583.363600000001</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2"/>
+      <c r="E5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="7">
+        <v>27880.991300000002</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6">
         <v>3</v>
       </c>
       <c r="C6" s="7">
         <v>18239.870999999999</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="7">
+        <v>30281.035100000001</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6">
         <v>4</v>
       </c>
       <c r="C7" s="7">
         <v>17230.960800000001</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="6">
         <v>10</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="7">
+        <v>32611.2016</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6">
         <v>5</v>
       </c>
       <c r="C8" s="7">
         <v>15962.530699999999</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9" s="7">
         <v>69538.666599999997</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6">
         <v>2</v>
       </c>
       <c r="C10" s="7">
         <v>67857.691500000001</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6">
         <v>3</v>
       </c>
       <c r="C11" s="7">
         <v>70084.654399999999</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6">
         <v>4</v>
       </c>
       <c r="C12" s="7">
         <v>67839.165099999998</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6">
         <v>5</v>
       </c>
       <c r="C13" s="7">
         <v>67676.634399999995</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>